<commit_message>
Adapted exampleTAS.xlsx to TAS structure
</commit_message>
<xml_diff>
--- a/ontology/examples/exampleTAS.xlsx
+++ b/ontology/examples/exampleTAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1129,9 +1129,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1143,6 +1140,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,10 +1485,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="4" t="s">
         <v>249</v>
       </c>
@@ -3007,31 +3007,31 @@
       <c r="B1" s="8">
         <v>2011</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
     </row>
     <row r="2" spans="1:30" ht="15.75">
       <c r="A2" s="6" t="s">
@@ -3040,81 +3040,81 @@
       <c r="B2" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
     </row>
     <row r="3" spans="1:30" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="25" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
     </row>
     <row r="4" spans="1:30">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>5</v>
       </c>
       <c r="D4" s="5">
@@ -3123,40 +3123,40 @@
       <c r="E4" s="5">
         <v>7</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27">
-        <f>AVERAGE(C4:E4)</f>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26">
+        <f t="shared" ref="G4:G9" si="0">AVERAGE(C4:E4)</f>
         <v>5</v>
       </c>
-      <c r="H4" s="27">
-        <f>STDEV(C4:E4)</f>
+      <c r="H4" s="26">
+        <f t="shared" ref="H4:H9" si="1">STDEV(C4:E4)</f>
         <v>2</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
     </row>
     <row r="5" spans="1:30">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -3168,40 +3168,40 @@
       <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27">
-        <f>AVERAGE(C5:E5)</f>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H5" s="27">
-        <f>STDEV(C5:E5)</f>
+      <c r="H5" s="26">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
     </row>
     <row r="6" spans="1:30">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -3214,40 +3214,40 @@
         <f>'2010-Raw'!E6*('2010-Raw'!E6/'2009-Raw'!E6)</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27">
-        <f>AVERAGE(C6:E6)</f>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26">
+        <f t="shared" si="0"/>
         <v>6.5555555555555545</v>
       </c>
-      <c r="H6" s="27">
-        <f>STDEV(C6:E6)</f>
+      <c r="H6" s="26">
+        <f t="shared" si="1"/>
         <v>3.8634085890474927</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
+      <c r="AD6" s="25"/>
     </row>
     <row r="7" spans="1:30">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -3259,40 +3259,40 @@
       <c r="E7" s="9">
         <v>8</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27">
-        <f>AVERAGE(C7:E7)</f>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26">
+        <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="H7" s="27">
-        <f>STDEV(C7:E7)</f>
+      <c r="H7" s="26">
+        <f t="shared" si="1"/>
         <v>2.309401076758502</v>
       </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="25"/>
+      <c r="AD7" s="25"/>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>244</v>
       </c>
       <c r="C8" s="9">
@@ -3304,40 +3304,40 @@
       <c r="E8" s="9">
         <v>8</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27">
-        <f>AVERAGE(C8:E8)</f>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H8" s="27">
-        <f>STDEV(C8:E8)</f>
+      <c r="H8" s="26">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
-      <c r="AD8" s="26"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="25"/>
+      <c r="AD8" s="25"/>
     </row>
     <row r="9" spans="1:30">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>255</v>
       </c>
       <c r="C9" s="9">
@@ -3349,37 +3349,37 @@
       <c r="E9" s="9">
         <v>4</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27">
-        <f>AVERAGE(C9:E9)</f>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26">
+        <f t="shared" si="0"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="H9" s="27">
-        <f>STDEV(C9:E9)</f>
+      <c r="H9" s="26">
+        <f t="shared" si="1"/>
         <v>2.0816659994661335</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AD9" s="25"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -3433,84 +3433,84 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>('2009-Sorted'!C4-'2009-Sorted'!G4)/'2009-Sorted'!H4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>('2009-Sorted'!D4-'2009-Sorted'!G4)/'2009-Sorted'!H4</f>
         <v>-1</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>('2009-Sorted'!E4-'2009-Sorted'!G4)/'2009-Sorted'!H4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <f>('2009-Sorted'!G5-'2009-Sorted'!C5)/'2009-Sorted'!H5</f>
         <v>-1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f>('2009-Sorted'!G5-'2009-Sorted'!D5)/'2009-Sorted'!H5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>('2009-Sorted'!G5-'2009-Sorted'!E5)/'2009-Sorted'!H5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <f>('2009-Sorted'!C6-'2009-Sorted'!G6)/'2009-Sorted'!H6</f>
         <v>-0.57735026918962551</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f>('2009-Sorted'!D6-'2009-Sorted'!G6)/'2009-Sorted'!H6</f>
         <v>-0.57735026918962551</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f>('2009-Sorted'!E6-'2009-Sorted'!G6)/'2009-Sorted'!H6</f>
         <v>1.1547005383792501</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <f>('2009-Sorted'!C7-'2009-Sorted'!G7)/'2009-Sorted'!H7</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <f>('2009-Sorted'!D7-'2009-Sorted'!G7)/'2009-Sorted'!H7</f>
         <v>-1.1547005383792521</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f>('2009-Sorted'!E7-'2009-Sorted'!G7)/'2009-Sorted'!H7</f>
         <v>0.57735026918962584</v>
       </c>
@@ -3574,84 +3574,84 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>('2010-Sorted'!C4-'2010-Sorted'!G4)/'2010-Sorted'!H4</f>
         <v>-0.21821789023599253</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>('2010-Sorted'!D4-'2010-Sorted'!G4)/'2010-Sorted'!H4</f>
         <v>-0.87287156094396978</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>('2010-Sorted'!E4-'2010-Sorted'!G4)/'2010-Sorted'!H4</f>
         <v>1.091089451179962</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <f>('2010-Sorted'!G5-'2010-Sorted'!C5)/'2010-Sorted'!H5</f>
         <v>-1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f>('2010-Sorted'!G5-'2010-Sorted'!D5)/'2010-Sorted'!H5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>('2010-Sorted'!G5-'2010-Sorted'!E5)/'2010-Sorted'!H5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <f>('2010-Sorted'!C6-'2010-Sorted'!G6)/'2010-Sorted'!H6</f>
         <v>-0.57735026918962584</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f>('2010-Sorted'!D6-'2010-Sorted'!G6)/'2010-Sorted'!H6</f>
         <v>-0.57735026918962584</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f>('2010-Sorted'!E6-'2010-Sorted'!G6)/'2010-Sorted'!H6</f>
         <v>1.1547005383792517</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <f>('2010-Sorted'!C7-'2010-Sorted'!G7)/'2010-Sorted'!H7</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <f>('2010-Sorted'!D7-'2010-Sorted'!G7)/'2010-Sorted'!H7</f>
         <v>-1.1547005383792517</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f>('2010-Sorted'!E7-'2010-Sorted'!G7)/'2010-Sorted'!H7</f>
         <v>0.57735026918962584</v>
       </c>
@@ -3715,101 +3715,101 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>('2011-Sorted'!C4-'2011-Sorted'!G4)/'2011-Sorted'!H4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>('2011-Sorted'!D4-'2011-Sorted'!G4)/'2011-Sorted'!H4</f>
         <v>-1</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>('2011-Sorted'!E4-'2011-Sorted'!G4)/'2011-Sorted'!H4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <f>('2011-Sorted'!G5-'2011-Sorted'!C5)/'2011-Sorted'!H5</f>
         <v>-1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f>('2011-Sorted'!G5-'2011-Sorted'!D5)/'2011-Sorted'!H5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>('2011-Sorted'!G5-'2011-Sorted'!E5)/'2011-Sorted'!H5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <f>('2011-Sorted'!C6-'2011-Sorted'!G6)/'2011-Sorted'!H6</f>
         <v>-0.92031569366888055</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f>('2011-Sorted'!D6-'2011-Sorted'!G6)/'2011-Sorted'!H6</f>
         <v>-0.14379932713576235</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f>('2011-Sorted'!E6-'2011-Sorted'!G6)/'2011-Sorted'!H6</f>
         <v>1.0641150208046437</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <f>('2011-Sorted'!C7-'2011-Sorted'!G7)/'2011-Sorted'!H7</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <f>('2011-Sorted'!D7-'2011-Sorted'!G7)/'2011-Sorted'!H7</f>
         <v>-1.1547005383792521</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f>('2011-Sorted'!E7-'2011-Sorted'!G7)/'2011-Sorted'!H7</f>
         <v>0.57735026918962584</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <f>('2011-Sorted'!C8-'2011-Sorted'!G8)/'2011-Sorted'!H8</f>
         <v>-1</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <f>('2011-Sorted'!D8-'2011-Sorted'!G8)/'2011-Sorted'!H8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f>('2011-Sorted'!E8-'2011-Sorted'!G8)/'2011-Sorted'!H8</f>
         <v>1</v>
       </c>
@@ -3818,18 +3818,18 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <f>('2011-Sorted'!C9-'2011-Sorted'!G9)/'2011-Sorted'!H9</f>
         <v>1.1208970766356094</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <f>('2011-Sorted'!D9-'2011-Sorted'!G9)/'2011-Sorted'!H9</f>
         <v>-0.80064076902543546</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <f>('2011-Sorted'!E9-'2011-Sorted'!G9)/'2011-Sorted'!H9</f>
         <v>-0.32025630761017432</v>
       </c>
@@ -3889,36 +3889,36 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>'2011-Normalized'!C4+8</f>
         <v>8</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>'2011-Normalized'!D4+8</f>
         <v>7</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>'2011-Normalized'!E4+8</f>
         <v>9</v>
       </c>
@@ -3926,91 +3926,91 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <f>'2011-Normalized'!C5+8</f>
         <v>7</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <f>'2011-Normalized'!D5+8</f>
         <v>8</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="27">
         <f>'2011-Normalized'!E5+8</f>
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <f>'2011-Normalized'!C6+8</f>
         <v>7.079684306331119</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f>'2011-Normalized'!D6+8</f>
         <v>7.8562006728642375</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f>'2011-Normalized'!E6+8</f>
         <v>9.0641150208046444</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <f>'2011-Normalized'!C7+8</f>
         <v>8.5773502691896262</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <f>'2011-Normalized'!D7+8</f>
         <v>6.8452994616207476</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f>'2011-Normalized'!E7+8</f>
         <v>8.5773502691896262</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>244</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <f>'2011-Normalized'!C8+8</f>
         <v>7</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <f>'2011-Normalized'!D8+8</f>
         <v>8</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f>'2011-Normalized'!E8+8</f>
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>255</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <f>'2011-Normalized'!C9+8</f>
         <v>9.1208970766356092</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <f>'2011-Normalized'!D9+8</f>
         <v>7.1993592309745642</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <f>'2011-Normalized'!E9+8</f>
         <v>7.6797436923898257</v>
       </c>
@@ -4080,41 +4080,41 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
       <c r="B4" s="7">
         <f>Metadata!C255</f>
         <v>1</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>'Indicators-Adjusted'!C4*B4</f>
         <v>8</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>'Indicators-Adjusted'!D4*B4</f>
         <v>7</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>'Indicators-Adjusted'!E4*B4</f>
         <v>9</v>
       </c>
@@ -4122,22 +4122,22 @@
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="B5" s="7">
         <f>Metadata!C256</f>
         <v>0.5</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <f>'Indicators-Adjusted'!C5*B5</f>
         <v>3.5</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f>'Indicators-Adjusted'!D5*B5</f>
         <v>4</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>'Indicators-Adjusted'!E5*B5</f>
         <v>4.5</v>
       </c>
@@ -4145,85 +4145,85 @@
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="B6" s="7">
         <f>Metadata!C257</f>
         <v>0.5</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <f>'Indicators-Adjusted'!C6*B6</f>
         <v>3.5398421531655595</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f>'Indicators-Adjusted'!D6*B6</f>
         <v>3.9281003364321188</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f>'Indicators-Adjusted'!E6*B6</f>
         <v>4.5320575104023222</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="B7" s="7">
         <f>Metadata!C258</f>
         <v>1</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <f>'Indicators-Adjusted'!C7*B7</f>
         <v>8.5773502691896262</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <f>'Indicators-Adjusted'!D7*B7</f>
         <v>6.8452994616207476</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f>'Indicators-Adjusted'!E7*B7</f>
         <v>8.5773502691896262</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>244</v>
       </c>
       <c r="B8" s="7">
         <f>Metadata!C259</f>
         <v>0.5</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <f>'Indicators-Adjusted'!C8*B8</f>
         <v>3.5</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <f>'Indicators-Adjusted'!D8*B8</f>
         <v>4</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f>'Indicators-Adjusted'!E8*B8</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>255</v>
       </c>
       <c r="B9" s="7">
         <f>Metadata!C260</f>
         <v>1</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <f>'Indicators-Adjusted'!C9*B9</f>
         <v>9.1208970766356092</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <f>'Indicators-Adjusted'!D9*B9</f>
         <v>7.1993592309745642</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <f>'Indicators-Adjusted'!E9*B9</f>
         <v>7.6797436923898257</v>
       </c>
@@ -4293,88 +4293,88 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>261</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>('Indicators-Weighted'!C4+'Indicators-Weighted'!C5)/2</f>
         <v>5.75</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>('Indicators-Weighted'!D4+'Indicators-Weighted'!D5)/2</f>
         <v>5.5</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>('Indicators-Weighted'!E4+'Indicators-Weighted'!E5)/2</f>
         <v>6.75</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>255</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <f>('Indicators-Weighted'!C9)</f>
         <v>9.1208970766356092</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f>('Indicators-Weighted'!D9)</f>
         <v>7.1993592309745642</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>('Indicators-Weighted'!E9)</f>
         <v>7.6797436923898257</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>270</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <f>('Indicators-Weighted'!C6)</f>
         <v>3.5398421531655595</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f>('Indicators-Weighted'!D6)</f>
         <v>3.9281003364321188</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f>('Indicators-Weighted'!E6)</f>
         <v>4.5320575104023222</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>262</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <f>('Indicators-Weighted'!C7+'Indicators-Weighted'!C8)/2</f>
         <v>6.0386751345948131</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <f>('Indicators-Weighted'!D7+'Indicators-Weighted'!D8)/2</f>
         <v>5.4226497308103738</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f>('Indicators-Weighted'!E7+'Indicators-Weighted'!E8)/2</f>
         <v>6.5386751345948131</v>
       </c>
@@ -4444,60 +4444,60 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>267</v>
       </c>
       <c r="B4" s="7">
         <f>Metadata!B270</f>
         <v>0.4</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>AVERAGE('Clusters-Weighted'!C4:'Clusters-Weighted'!C5)</f>
         <v>7.4354485383178046</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>AVERAGE('Clusters-Weighted'!D4:'Clusters-Weighted'!D5)</f>
         <v>6.3496796154872825</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>AVERAGE('Clusters-Weighted'!E4:'Clusters-Weighted'!E5)</f>
         <v>7.2148718461949128</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>268</v>
       </c>
       <c r="B5" s="7">
         <f>Metadata!B271</f>
         <v>0.6</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <f>AVERAGE('Clusters-Weighted'!C6:'Clusters-Weighted'!C7)</f>
         <v>4.7892586438801867</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f>AVERAGE('Clusters-Weighted'!D6:'Clusters-Weighted'!D7)</f>
         <v>4.6753750336212461</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>AVERAGE('Clusters-Weighted'!E6:'Clusters-Weighted'!E7)</f>
         <v>5.5353663224985681</v>
       </c>
@@ -4567,34 +4567,34 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>272</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>'Subindex-Weighted'!C4*'Subindex-Weighted'!B4+'Subindex-Weighted'!C5*'Subindex-Weighted'!B5</f>
         <v>5.8477346016552341</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>'Subindex-Weighted'!D4*'Subindex-Weighted'!B4+'Subindex-Weighted'!D5*'Subindex-Weighted'!B5</f>
         <v>5.3450968663676601</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>'Subindex-Weighted'!E4*'Subindex-Weighted'!B4+'Subindex-Weighted'!E5*'Subindex-Weighted'!B5</f>
         <v>6.2071685319771062</v>
       </c>
@@ -4620,7 +4620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -4781,7 +4781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4793,7 +4793,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="8">
@@ -4801,7 +4801,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>246</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -4809,28 +4809,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>2</v>
       </c>
       <c r="D4" s="5">
@@ -4844,7 +4844,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -4861,7 +4861,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -4878,7 +4878,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -4937,7 +4937,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="8">
@@ -4945,7 +4945,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>246</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -4953,28 +4953,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>3</v>
       </c>
       <c r="E4" s="5">
@@ -4983,7 +4983,7 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -4998,7 +4998,7 @@
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -5010,7 +5010,7 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -5083,28 +5083,28 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>5</v>
       </c>
       <c r="D4" s="5">
@@ -5118,7 +5118,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -5137,7 +5137,7 @@
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -5153,7 +5153,7 @@
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -5172,7 +5172,7 @@
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>244</v>
       </c>
       <c r="C8" s="9">
@@ -5191,7 +5191,7 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>255</v>
       </c>
       <c r="C9" s="9">
@@ -5259,28 +5259,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>2</v>
       </c>
       <c r="D4" s="5">
@@ -5294,7 +5294,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -5311,7 +5311,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -5328,7 +5328,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -5396,28 +5396,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>3</v>
       </c>
       <c r="D4" s="10">
@@ -5433,7 +5433,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -5451,7 +5451,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -5470,7 +5470,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -5546,28 +5546,28 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>5</v>
       </c>
       <c r="D4" s="5">
@@ -5581,7 +5581,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -5600,7 +5600,7 @@
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -5620,7 +5620,7 @@
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -5639,7 +5639,7 @@
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>244</v>
       </c>
       <c r="C8" s="9">
@@ -5658,7 +5658,7 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>255</v>
       </c>
       <c r="C9" s="9">
@@ -5728,117 +5728,117 @@
       </c>
     </row>
     <row r="3" spans="1:93" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="25" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
-      <c r="AH3" s="24"/>
-      <c r="AI3" s="24"/>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="24"/>
-      <c r="AN3" s="24"/>
-      <c r="AO3" s="24"/>
-      <c r="AP3" s="24"/>
-      <c r="AQ3" s="24"/>
-      <c r="AR3" s="24"/>
-      <c r="AS3" s="24"/>
-      <c r="AT3" s="24"/>
-      <c r="AU3" s="24"/>
-      <c r="AV3" s="24"/>
-      <c r="AW3" s="24"/>
-      <c r="AX3" s="24"/>
-      <c r="AY3" s="24"/>
-      <c r="AZ3" s="24"/>
-      <c r="BA3" s="24"/>
-      <c r="BB3" s="24"/>
-      <c r="BC3" s="24"/>
-      <c r="BD3" s="24"/>
-      <c r="BE3" s="24"/>
-      <c r="BF3" s="24"/>
-      <c r="BG3" s="24"/>
-      <c r="BH3" s="24"/>
-      <c r="BI3" s="24"/>
-      <c r="BJ3" s="24"/>
-      <c r="BK3" s="24"/>
-      <c r="BL3" s="24"/>
-      <c r="BM3" s="24"/>
-      <c r="BN3" s="24"/>
-      <c r="BO3" s="24"/>
-      <c r="BP3" s="24"/>
-      <c r="BQ3" s="24"/>
-      <c r="BR3" s="24"/>
-      <c r="BS3" s="24"/>
-      <c r="BT3" s="24"/>
-      <c r="BU3" s="24"/>
-      <c r="BV3" s="24"/>
-      <c r="BW3" s="24"/>
-      <c r="BX3" s="24"/>
-      <c r="BY3" s="24"/>
-      <c r="BZ3" s="24"/>
-      <c r="CA3" s="24"/>
-      <c r="CB3" s="24"/>
-      <c r="CC3" s="24"/>
-      <c r="CD3" s="24"/>
-      <c r="CE3" s="24"/>
-      <c r="CF3" s="24"/>
-      <c r="CG3" s="24"/>
-      <c r="CH3" s="24"/>
-      <c r="CI3" s="24"/>
-      <c r="CJ3" s="24"/>
-      <c r="CK3" s="24"/>
-      <c r="CL3" s="24"/>
-      <c r="CM3" s="24"/>
-      <c r="CN3" s="24"/>
-      <c r="CO3" s="24"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23"/>
+      <c r="AX3" s="23"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="23"/>
+      <c r="BE3" s="23"/>
+      <c r="BF3" s="23"/>
+      <c r="BG3" s="23"/>
+      <c r="BH3" s="23"/>
+      <c r="BI3" s="23"/>
+      <c r="BJ3" s="23"/>
+      <c r="BK3" s="23"/>
+      <c r="BL3" s="23"/>
+      <c r="BM3" s="23"/>
+      <c r="BN3" s="23"/>
+      <c r="BO3" s="23"/>
+      <c r="BP3" s="23"/>
+      <c r="BQ3" s="23"/>
+      <c r="BR3" s="23"/>
+      <c r="BS3" s="23"/>
+      <c r="BT3" s="23"/>
+      <c r="BU3" s="23"/>
+      <c r="BV3" s="23"/>
+      <c r="BW3" s="23"/>
+      <c r="BX3" s="23"/>
+      <c r="BY3" s="23"/>
+      <c r="BZ3" s="23"/>
+      <c r="CA3" s="23"/>
+      <c r="CB3" s="23"/>
+      <c r="CC3" s="23"/>
+      <c r="CD3" s="23"/>
+      <c r="CE3" s="23"/>
+      <c r="CF3" s="23"/>
+      <c r="CG3" s="23"/>
+      <c r="CH3" s="23"/>
+      <c r="CI3" s="23"/>
+      <c r="CJ3" s="23"/>
+      <c r="CK3" s="23"/>
+      <c r="CL3" s="23"/>
+      <c r="CM3" s="23"/>
+      <c r="CN3" s="23"/>
+      <c r="CO3" s="23"/>
     </row>
     <row r="4" spans="1:93">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>2</v>
       </c>
       <c r="D4" s="5">
@@ -5858,7 +5858,7 @@
       </c>
     </row>
     <row r="5" spans="1:93">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -5881,7 +5881,7 @@
       </c>
     </row>
     <row r="6" spans="1:93">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -5904,7 +5904,7 @@
       </c>
     </row>
     <row r="7" spans="1:93">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -5977,22 +5977,22 @@
       <c r="B1" s="8">
         <v>2010</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
     </row>
     <row r="2" spans="1:21" ht="15.75">
       <c r="A2" s="6" t="s">
@@ -6001,63 +6001,63 @@
       <c r="B2" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
     </row>
     <row r="3" spans="1:21" s="6" customFormat="1" ht="15.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="25" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>3</v>
       </c>
       <c r="D4" s="10">
@@ -6067,31 +6067,31 @@
       <c r="E4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27">
+      <c r="F4" s="26"/>
+      <c r="G4" s="26">
         <f>AVERAGE(C4:E4)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="26">
         <f>STDEV(C4:E4)</f>
         <v>1.5275252316519463</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="5">
@@ -6103,31 +6103,31 @@
       <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27">
+      <c r="F5" s="26"/>
+      <c r="G5" s="26">
         <f>AVERAGE(C5:E5)</f>
         <v>6</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <f>STDEV(C5:E5)</f>
         <v>2</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C6" s="5">
@@ -6140,31 +6140,31 @@
       <c r="E6" s="5">
         <v>8</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27">
+      <c r="F6" s="26"/>
+      <c r="G6" s="26">
         <f>AVERAGE(C6:E6)</f>
         <v>6</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <f>STDEV(C6:E6)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>254</v>
       </c>
       <c r="C7" s="9">
@@ -6176,28 +6176,28 @@
       <c r="E7" s="9">
         <v>6</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27">
+      <c r="F7" s="26"/>
+      <c r="G7" s="26">
         <f>AVERAGE(C7:E7)</f>
         <v>5</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="26">
         <f>STDEV(C7:E7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="15"/>

</xml_diff>